<commit_message>
fixed small error in the previous commit
</commit_message>
<xml_diff>
--- a/Databases/한국어_sentences.xlsx
+++ b/Databases/한국어_sentences.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23426"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Me\Documents\GitHub Clones\anki-card-importer\Databases\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FC24223-DB9A-4D9F-8C44-79E8AC1DE45C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14220" yWindow="15480" windowWidth="13170" windowHeight="13260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="sentences" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -1635,8 +1629,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1699,14 +1693,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -1753,7 +1739,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1785,27 +1771,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1837,24 +1805,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2030,16 +1980,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D242"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A220" workbookViewId="0">
-      <selection activeCell="J231" sqref="J231"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2053,7 +2001,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -2067,7 +2015,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -2081,7 +2029,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -2095,7 +2043,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -2109,7 +2057,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -2123,7 +2071,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -2137,7 +2085,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -2151,7 +2099,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -2165,7 +2113,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -2179,7 +2127,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -2193,7 +2141,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -2207,7 +2155,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -2221,7 +2169,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -2235,7 +2183,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -2249,7 +2197,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -2263,7 +2211,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -2277,7 +2225,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -2291,7 +2239,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4">
       <c r="A19" t="s">
         <v>21</v>
       </c>
@@ -2305,7 +2253,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4">
       <c r="A20" t="s">
         <v>22</v>
       </c>
@@ -2319,7 +2267,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4">
       <c r="A21" t="s">
         <v>23</v>
       </c>
@@ -2333,7 +2281,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4">
       <c r="A22" t="s">
         <v>24</v>
       </c>
@@ -2347,7 +2295,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4">
       <c r="A23" t="s">
         <v>25</v>
       </c>
@@ -2361,7 +2309,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4">
       <c r="A24" t="s">
         <v>26</v>
       </c>
@@ -2375,7 +2323,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4">
       <c r="A25" t="s">
         <v>27</v>
       </c>
@@ -2389,7 +2337,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4">
       <c r="A26" t="s">
         <v>28</v>
       </c>
@@ -2403,7 +2351,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4">
       <c r="A27" t="s">
         <v>5</v>
       </c>
@@ -2417,7 +2365,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4">
       <c r="A28" t="s">
         <v>29</v>
       </c>
@@ -2431,7 +2379,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4">
       <c r="A29" t="s">
         <v>30</v>
       </c>
@@ -2445,7 +2393,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4">
       <c r="A30" t="s">
         <v>31</v>
       </c>
@@ -2459,7 +2407,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4">
       <c r="A31" t="s">
         <v>32</v>
       </c>
@@ -2473,7 +2421,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4">
       <c r="A32" t="s">
         <v>33</v>
       </c>
@@ -2487,7 +2435,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4">
       <c r="A33" t="s">
         <v>34</v>
       </c>
@@ -2501,7 +2449,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4">
       <c r="A34" t="s">
         <v>35</v>
       </c>
@@ -2515,7 +2463,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4">
       <c r="A35" t="s">
         <v>36</v>
       </c>
@@ -2529,7 +2477,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4">
       <c r="A36" t="s">
         <v>37</v>
       </c>
@@ -2543,7 +2491,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4">
       <c r="A37" t="s">
         <v>38</v>
       </c>
@@ -2557,7 +2505,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4">
       <c r="A38" t="s">
         <v>39</v>
       </c>
@@ -2571,7 +2519,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4">
       <c r="A39" t="s">
         <v>40</v>
       </c>
@@ -2585,7 +2533,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4">
       <c r="A40" t="s">
         <v>41</v>
       </c>
@@ -2599,7 +2547,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4">
       <c r="A41" t="s">
         <v>42</v>
       </c>
@@ -2613,7 +2561,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4">
       <c r="A42" t="s">
         <v>43</v>
       </c>
@@ -2627,7 +2575,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4">
       <c r="A43" t="s">
         <v>44</v>
       </c>
@@ -2641,7 +2589,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4">
       <c r="A44" t="s">
         <v>45</v>
       </c>
@@ -2655,7 +2603,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4">
       <c r="A45" t="s">
         <v>46</v>
       </c>
@@ -2669,7 +2617,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4">
       <c r="A46" t="s">
         <v>47</v>
       </c>
@@ -2683,7 +2631,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4">
       <c r="A47" t="s">
         <v>48</v>
       </c>
@@ -2697,7 +2645,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4">
       <c r="A48" t="s">
         <v>49</v>
       </c>
@@ -2711,7 +2659,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4">
       <c r="A49" t="s">
         <v>50</v>
       </c>
@@ -2725,7 +2673,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4">
       <c r="A50" t="s">
         <v>51</v>
       </c>
@@ -2739,7 +2687,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4">
       <c r="A51" t="s">
         <v>49</v>
       </c>
@@ -2753,7 +2701,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4">
       <c r="A52" t="s">
         <v>50</v>
       </c>
@@ -2767,7 +2715,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4">
       <c r="A53" t="s">
         <v>52</v>
       </c>
@@ -2781,7 +2729,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4">
       <c r="A54" t="s">
         <v>53</v>
       </c>
@@ -2795,7 +2743,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4">
       <c r="A55" t="s">
         <v>54</v>
       </c>
@@ -2809,7 +2757,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4">
       <c r="A56" t="s">
         <v>55</v>
       </c>
@@ -2823,7 +2771,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4">
       <c r="A57" t="s">
         <v>56</v>
       </c>
@@ -2837,7 +2785,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4">
       <c r="A58" t="s">
         <v>7</v>
       </c>
@@ -2851,7 +2799,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4">
       <c r="A59" t="s">
         <v>57</v>
       </c>
@@ -2865,7 +2813,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4">
       <c r="A60" t="s">
         <v>9</v>
       </c>
@@ -2879,7 +2827,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4">
       <c r="A61" t="s">
         <v>58</v>
       </c>
@@ -2893,7 +2841,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4">
       <c r="A62" t="s">
         <v>59</v>
       </c>
@@ -2907,7 +2855,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4">
       <c r="A63" t="s">
         <v>60</v>
       </c>
@@ -2921,7 +2869,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4">
       <c r="A64" t="s">
         <v>61</v>
       </c>
@@ -2935,7 +2883,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4">
       <c r="A65" t="s">
         <v>62</v>
       </c>
@@ -2949,7 +2897,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4">
       <c r="A66" t="s">
         <v>10</v>
       </c>
@@ -2963,7 +2911,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4">
       <c r="A67" t="s">
         <v>63</v>
       </c>
@@ -2977,7 +2925,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4">
       <c r="A68" t="s">
         <v>64</v>
       </c>
@@ -2991,7 +2939,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4">
       <c r="A69" t="s">
         <v>12</v>
       </c>
@@ -3005,7 +2953,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4">
       <c r="A70" t="s">
         <v>65</v>
       </c>
@@ -3019,7 +2967,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4">
       <c r="A71" t="s">
         <v>66</v>
       </c>
@@ -3033,7 +2981,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4">
       <c r="A72" t="s">
         <v>67</v>
       </c>
@@ -3047,7 +2995,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4">
       <c r="A73" t="s">
         <v>68</v>
       </c>
@@ -3061,7 +3009,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4">
       <c r="A74" t="s">
         <v>69</v>
       </c>
@@ -3075,7 +3023,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4">
       <c r="A75" t="s">
         <v>70</v>
       </c>
@@ -3089,7 +3037,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4">
       <c r="A76" t="s">
         <v>71</v>
       </c>
@@ -3103,7 +3051,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4">
       <c r="A77" t="s">
         <v>72</v>
       </c>
@@ -3117,7 +3065,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4">
       <c r="A78" t="s">
         <v>73</v>
       </c>
@@ -3131,7 +3079,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4">
       <c r="A79" t="s">
         <v>74</v>
       </c>
@@ -3145,7 +3093,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4">
       <c r="A80" t="s">
         <v>75</v>
       </c>
@@ -3159,7 +3107,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4">
       <c r="A81" t="s">
         <v>76</v>
       </c>
@@ -3173,7 +3121,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4">
       <c r="A82" t="s">
         <v>77</v>
       </c>
@@ -3187,7 +3135,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4">
       <c r="A83" t="s">
         <v>78</v>
       </c>
@@ -3201,7 +3149,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4">
       <c r="A84" t="s">
         <v>16</v>
       </c>
@@ -3215,7 +3163,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4">
       <c r="A85" t="s">
         <v>79</v>
       </c>
@@ -3229,7 +3177,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4">
       <c r="A86" t="s">
         <v>80</v>
       </c>
@@ -3243,7 +3191,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4">
       <c r="A87" t="s">
         <v>81</v>
       </c>
@@ -3257,7 +3205,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4">
       <c r="A88" t="s">
         <v>82</v>
       </c>
@@ -3271,7 +3219,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4">
       <c r="A89" t="s">
         <v>83</v>
       </c>
@@ -3285,7 +3233,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4">
       <c r="A90" t="s">
         <v>84</v>
       </c>
@@ -3299,7 +3247,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4">
       <c r="A91" t="s">
         <v>85</v>
       </c>
@@ -3313,7 +3261,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4">
       <c r="A92" t="s">
         <v>86</v>
       </c>
@@ -3327,7 +3275,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4">
       <c r="A93" t="s">
         <v>18</v>
       </c>
@@ -3341,7 +3289,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4">
       <c r="A94" t="s">
         <v>87</v>
       </c>
@@ -3355,7 +3303,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4">
       <c r="A95" t="s">
         <v>88</v>
       </c>
@@ -3369,7 +3317,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4">
       <c r="A96" t="s">
         <v>89</v>
       </c>
@@ -3383,7 +3331,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4">
       <c r="A97" t="s">
         <v>90</v>
       </c>
@@ -3397,7 +3345,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4">
       <c r="A98" t="s">
         <v>91</v>
       </c>
@@ -3411,7 +3359,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:4">
       <c r="A99" t="s">
         <v>92</v>
       </c>
@@ -3425,7 +3373,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4">
       <c r="A100" t="s">
         <v>93</v>
       </c>
@@ -3439,7 +3387,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4">
       <c r="A101" t="s">
         <v>94</v>
       </c>
@@ -3453,7 +3401,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4">
       <c r="A102" t="s">
         <v>95</v>
       </c>
@@ -3467,7 +3415,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4">
       <c r="A103" t="s">
         <v>96</v>
       </c>
@@ -3481,7 +3429,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4">
       <c r="A104" t="s">
         <v>97</v>
       </c>
@@ -3495,7 +3443,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:4">
       <c r="A105" t="s">
         <v>98</v>
       </c>
@@ -3509,7 +3457,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:4">
       <c r="A106" t="s">
         <v>99</v>
       </c>
@@ -3523,7 +3471,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:4">
       <c r="A107" t="s">
         <v>100</v>
       </c>
@@ -3537,7 +3485,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:4">
       <c r="A108" t="s">
         <v>101</v>
       </c>
@@ -3551,7 +3499,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:4">
       <c r="A109" t="s">
         <v>102</v>
       </c>
@@ -3565,7 +3513,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:4">
       <c r="A110" t="s">
         <v>103</v>
       </c>
@@ -3579,7 +3527,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:4">
       <c r="A111" t="s">
         <v>24</v>
       </c>
@@ -3593,7 +3541,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:4">
       <c r="A112" t="s">
         <v>104</v>
       </c>
@@ -3607,7 +3555,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:4">
       <c r="A113" t="s">
         <v>105</v>
       </c>
@@ -3621,7 +3569,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:4">
       <c r="A114" t="s">
         <v>28</v>
       </c>
@@ -3635,7 +3583,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:4">
       <c r="A115" t="s">
         <v>106</v>
       </c>
@@ -3649,7 +3597,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:4">
       <c r="A116" t="s">
         <v>107</v>
       </c>
@@ -3663,7 +3611,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:4">
       <c r="A117" t="s">
         <v>108</v>
       </c>
@@ -3677,7 +3625,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:4">
       <c r="A118" t="s">
         <v>109</v>
       </c>
@@ -3691,7 +3639,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:4">
       <c r="A119" t="s">
         <v>110</v>
       </c>
@@ -3705,7 +3653,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:4">
       <c r="A120" t="s">
         <v>111</v>
       </c>
@@ -3719,7 +3667,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:4">
       <c r="A121" t="s">
         <v>28</v>
       </c>
@@ -3733,7 +3681,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:4">
       <c r="A122" t="s">
         <v>112</v>
       </c>
@@ -3747,7 +3695,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:4">
       <c r="A123" t="s">
         <v>113</v>
       </c>
@@ -3761,7 +3709,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:4">
       <c r="A124" t="s">
         <v>114</v>
       </c>
@@ -3775,7 +3723,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:4">
       <c r="A125" t="s">
         <v>115</v>
       </c>
@@ -3789,7 +3737,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:4">
       <c r="A126" t="s">
         <v>116</v>
       </c>
@@ -3803,7 +3751,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:4">
       <c r="A127" t="s">
         <v>117</v>
       </c>
@@ -3817,7 +3765,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:4">
       <c r="A128" t="s">
         <v>118</v>
       </c>
@@ -3831,7 +3779,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:4">
       <c r="A129" t="s">
         <v>119</v>
       </c>
@@ -3845,7 +3793,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:4">
       <c r="A130" t="s">
         <v>120</v>
       </c>
@@ -3859,7 +3807,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:4">
       <c r="A131" t="s">
         <v>121</v>
       </c>
@@ -3873,7 +3821,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:4">
       <c r="A132" t="s">
         <v>122</v>
       </c>
@@ -3887,7 +3835,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:4">
       <c r="A133" t="s">
         <v>123</v>
       </c>
@@ -3901,7 +3849,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:4">
       <c r="A134" t="s">
         <v>124</v>
       </c>
@@ -3915,7 +3863,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:4">
       <c r="A135" t="s">
         <v>125</v>
       </c>
@@ -3929,7 +3877,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:4">
       <c r="A136" t="s">
         <v>126</v>
       </c>
@@ -3943,7 +3891,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:4">
       <c r="A137" t="s">
         <v>127</v>
       </c>
@@ -3957,7 +3905,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:4">
       <c r="A138" t="s">
         <v>128</v>
       </c>
@@ -3971,7 +3919,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:4">
       <c r="A139" t="s">
         <v>129</v>
       </c>
@@ -3985,7 +3933,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:4">
       <c r="A140" t="s">
         <v>130</v>
       </c>
@@ -3999,7 +3947,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:4">
       <c r="A141" t="s">
         <v>131</v>
       </c>
@@ -4013,7 +3961,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:4">
       <c r="A142" t="s">
         <v>31</v>
       </c>
@@ -4027,7 +3975,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:4">
       <c r="A143" t="s">
         <v>132</v>
       </c>
@@ -4041,7 +3989,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:4">
       <c r="A144" t="s">
         <v>133</v>
       </c>
@@ -4055,7 +4003,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:4">
       <c r="A145" t="s">
         <v>134</v>
       </c>
@@ -4069,7 +4017,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:4">
       <c r="A146" t="s">
         <v>135</v>
       </c>
@@ -4083,7 +4031,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:4">
       <c r="A147" t="s">
         <v>136</v>
       </c>
@@ -4097,7 +4045,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:4">
       <c r="A148" t="s">
         <v>137</v>
       </c>
@@ -4111,7 +4059,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:4">
       <c r="A149" t="s">
         <v>138</v>
       </c>
@@ -4125,7 +4073,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:4">
       <c r="A150" t="s">
         <v>139</v>
       </c>
@@ -4139,7 +4087,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:4">
       <c r="A151" t="s">
         <v>140</v>
       </c>
@@ -4153,7 +4101,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:4">
       <c r="A152" t="s">
         <v>141</v>
       </c>
@@ -4167,7 +4115,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:4">
       <c r="A153" t="s">
         <v>34</v>
       </c>
@@ -4181,7 +4129,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:4">
       <c r="A154" t="s">
         <v>142</v>
       </c>
@@ -4195,7 +4143,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:4">
       <c r="A155" t="s">
         <v>143</v>
       </c>
@@ -4209,7 +4157,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:4">
       <c r="A156" t="s">
         <v>144</v>
       </c>
@@ -4223,7 +4171,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:4">
       <c r="A157" t="s">
         <v>34</v>
       </c>
@@ -4237,7 +4185,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:4">
       <c r="A158" t="s">
         <v>145</v>
       </c>
@@ -4251,7 +4199,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:4">
       <c r="A159" t="s">
         <v>146</v>
       </c>
@@ -4265,7 +4213,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:4">
       <c r="A160" t="s">
         <v>146</v>
       </c>
@@ -4279,7 +4227,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:4">
       <c r="A161" t="s">
         <v>147</v>
       </c>
@@ -4293,7 +4241,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:4">
       <c r="A162" t="s">
         <v>148</v>
       </c>
@@ -4307,7 +4255,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:4">
       <c r="A163" t="s">
         <v>149</v>
       </c>
@@ -4321,7 +4269,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:4">
       <c r="A164" t="s">
         <v>150</v>
       </c>
@@ -4335,7 +4283,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:4">
       <c r="A165" t="s">
         <v>151</v>
       </c>
@@ -4349,7 +4297,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:4">
       <c r="A166" t="s">
         <v>152</v>
       </c>
@@ -4363,7 +4311,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:4">
       <c r="A167" t="s">
         <v>153</v>
       </c>
@@ -4377,7 +4325,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:4">
       <c r="A168" t="s">
         <v>154</v>
       </c>
@@ -4391,7 +4339,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:4">
       <c r="A169" t="s">
         <v>155</v>
       </c>
@@ -4405,7 +4353,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:4">
       <c r="A170" t="s">
         <v>156</v>
       </c>
@@ -4419,7 +4367,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:4">
       <c r="A171" t="s">
         <v>157</v>
       </c>
@@ -4433,7 +4381,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:4">
       <c r="A172" t="s">
         <v>158</v>
       </c>
@@ -4447,7 +4395,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:4">
       <c r="A173" t="s">
         <v>159</v>
       </c>
@@ -4461,7 +4409,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:4">
       <c r="A174" t="s">
         <v>160</v>
       </c>
@@ -4475,7 +4423,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:4">
       <c r="A175" t="s">
         <v>161</v>
       </c>
@@ -4489,7 +4437,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:4">
       <c r="A176" t="s">
         <v>162</v>
       </c>
@@ -4503,7 +4451,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:4">
       <c r="A177" t="s">
         <v>163</v>
       </c>
@@ -4517,7 +4465,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:4">
       <c r="A178" t="s">
         <v>164</v>
       </c>
@@ -4531,7 +4479,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:4">
       <c r="A179" t="s">
         <v>165</v>
       </c>
@@ -4545,7 +4493,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:4">
       <c r="A180" t="s">
         <v>166</v>
       </c>
@@ -4559,7 +4507,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:4">
       <c r="A181" t="s">
         <v>38</v>
       </c>
@@ -4573,7 +4521,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:4">
       <c r="A182" t="s">
         <v>167</v>
       </c>
@@ -4587,7 +4535,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:4">
       <c r="A183" t="s">
         <v>168</v>
       </c>
@@ -4601,7 +4549,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:4">
       <c r="A184" t="s">
         <v>169</v>
       </c>
@@ -4615,7 +4563,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:4">
       <c r="A185" t="s">
         <v>170</v>
       </c>
@@ -4629,7 +4577,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:4">
       <c r="A186" t="s">
         <v>171</v>
       </c>
@@ -4643,7 +4591,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:4">
       <c r="A187" t="s">
         <v>172</v>
       </c>
@@ -4657,7 +4605,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:4">
       <c r="A188" t="s">
         <v>173</v>
       </c>
@@ -4671,7 +4619,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:4">
       <c r="A189" t="s">
         <v>174</v>
       </c>
@@ -4685,7 +4633,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:4">
       <c r="A190" t="s">
         <v>39</v>
       </c>
@@ -4699,7 +4647,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:4">
       <c r="A191" t="s">
         <v>175</v>
       </c>
@@ -4713,7 +4661,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:4">
       <c r="A192" t="s">
         <v>176</v>
       </c>
@@ -4727,7 +4675,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:4">
       <c r="A193" t="s">
         <v>177</v>
       </c>
@@ -4741,7 +4689,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:4">
       <c r="A194" t="s">
         <v>178</v>
       </c>
@@ -4755,7 +4703,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:4">
       <c r="A195" t="s">
         <v>179</v>
       </c>
@@ -4769,7 +4717,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:4">
       <c r="A196" t="s">
         <v>180</v>
       </c>
@@ -4783,7 +4731,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:4">
       <c r="A197" t="s">
         <v>181</v>
       </c>
@@ -4797,7 +4745,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:4">
       <c r="A198" t="s">
         <v>182</v>
       </c>
@@ -4811,7 +4759,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:4">
       <c r="A199" t="s">
         <v>183</v>
       </c>
@@ -4825,7 +4773,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:4">
       <c r="A200" t="s">
         <v>184</v>
       </c>
@@ -4839,7 +4787,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:4">
       <c r="A201" t="s">
         <v>185</v>
       </c>
@@ -4853,7 +4801,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:4">
       <c r="A202" t="s">
         <v>186</v>
       </c>
@@ -4867,7 +4815,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:4">
       <c r="A203" t="s">
         <v>187</v>
       </c>
@@ -4881,7 +4829,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:4">
       <c r="A204" t="s">
         <v>188</v>
       </c>
@@ -4895,7 +4843,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:4">
       <c r="A205" t="s">
         <v>189</v>
       </c>
@@ -4909,7 +4857,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="206" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:4">
       <c r="A206" t="s">
         <v>190</v>
       </c>
@@ -4923,7 +4871,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="207" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:4">
       <c r="A207" t="s">
         <v>43</v>
       </c>
@@ -4937,7 +4885,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="208" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:4">
       <c r="A208" t="s">
         <v>191</v>
       </c>
@@ -4951,7 +4899,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="209" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:4">
       <c r="A209" t="s">
         <v>192</v>
       </c>
@@ -4965,7 +4913,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="210" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:4">
       <c r="A210" t="s">
         <v>193</v>
       </c>
@@ -4979,7 +4927,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:4">
       <c r="A211" t="s">
         <v>194</v>
       </c>
@@ -4993,7 +4941,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="212" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:4">
       <c r="A212" t="s">
         <v>43</v>
       </c>
@@ -5007,7 +4955,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="213" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:4">
       <c r="A213" t="s">
         <v>195</v>
       </c>
@@ -5021,7 +4969,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="214" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:4">
       <c r="A214" t="s">
         <v>196</v>
       </c>
@@ -5035,7 +4983,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="215" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:4">
       <c r="A215" t="s">
         <v>197</v>
       </c>
@@ -5049,7 +4997,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="216" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:4">
       <c r="A216" t="s">
         <v>198</v>
       </c>
@@ -5063,7 +5011,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="217" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:4">
       <c r="A217" t="s">
         <v>199</v>
       </c>
@@ -5077,7 +5025,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="218" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:4">
       <c r="A218" t="s">
         <v>200</v>
       </c>
@@ -5091,7 +5039,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="219" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:4">
       <c r="A219" t="s">
         <v>201</v>
       </c>
@@ -5105,7 +5053,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="220" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:4">
       <c r="A220" t="s">
         <v>202</v>
       </c>
@@ -5119,7 +5067,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="221" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:4">
       <c r="A221" t="s">
         <v>203</v>
       </c>
@@ -5133,7 +5081,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="222" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:4">
       <c r="A222" t="s">
         <v>204</v>
       </c>
@@ -5147,7 +5095,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="223" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:4">
       <c r="A223" t="s">
         <v>205</v>
       </c>
@@ -5161,7 +5109,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="224" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:4">
       <c r="A224" t="s">
         <v>46</v>
       </c>
@@ -5175,7 +5123,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="225" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:4">
       <c r="A225" t="s">
         <v>206</v>
       </c>
@@ -5189,7 +5137,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="226" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:4">
       <c r="A226" t="s">
         <v>207</v>
       </c>
@@ -5203,7 +5151,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="227" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:4">
       <c r="A227" t="s">
         <v>208</v>
       </c>
@@ -5217,7 +5165,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="228" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:4">
       <c r="A228" t="s">
         <v>209</v>
       </c>
@@ -5231,7 +5179,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="229" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:4">
       <c r="A229" t="s">
         <v>210</v>
       </c>
@@ -5245,7 +5193,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="230" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:4">
       <c r="A230" t="s">
         <v>211</v>
       </c>
@@ -5259,7 +5207,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="231" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:4">
       <c r="A231" t="s">
         <v>212</v>
       </c>
@@ -5273,7 +5221,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="232" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:4">
       <c r="A232" t="s">
         <v>213</v>
       </c>
@@ -5287,7 +5235,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="233" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:4">
       <c r="A233" t="s">
         <v>214</v>
       </c>
@@ -5301,7 +5249,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="234" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:4">
       <c r="A234" t="s">
         <v>215</v>
       </c>
@@ -5315,7 +5263,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="235" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:4">
       <c r="A235" t="s">
         <v>216</v>
       </c>
@@ -5329,7 +5277,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="236" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:4">
       <c r="A236" t="s">
         <v>217</v>
       </c>
@@ -5343,7 +5291,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="237" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:4">
       <c r="A237" t="s">
         <v>218</v>
       </c>
@@ -5357,7 +5305,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="238" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:4">
       <c r="A238" t="s">
         <v>219</v>
       </c>
@@ -5371,7 +5319,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="239" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:4">
       <c r="A239" t="s">
         <v>220</v>
       </c>
@@ -5385,7 +5333,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="240" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:4">
       <c r="A240" t="s">
         <v>221</v>
       </c>
@@ -5399,7 +5347,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="241" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:4">
       <c r="A241" t="s">
         <v>222</v>
       </c>
@@ -5413,7 +5361,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="242" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:4">
       <c r="A242" t="s">
         <v>223</v>
       </c>

</xml_diff>